<commit_message>
populate rows from input file to output file
</commit_message>
<xml_diff>
--- a/build/resources/test/Input.xlsx
+++ b/build/resources/test/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\7.AUTOMATION\FillDataInSpreadSheet\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4197B06E-6866-4D6F-B282-1289D5D1A4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2025A7AD-13BF-45D7-9398-139CAB6D4A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>yolima</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>hola</t>
+  </si>
+  <si>
+    <t>ggg</t>
+  </si>
+  <si>
+    <t>rr</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -351,15 +363,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -372,33 +384,28 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duplication of records up to a limit
</commit_message>
<xml_diff>
--- a/build/resources/test/Input.xlsx
+++ b/build/resources/test/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\7.AUTOMATION\FillDataInSpreadSheet\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2025A7AD-13BF-45D7-9398-139CAB6D4A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F203A470-21E9-4C7D-9B06-433244C9A97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
-  <si>
-    <t>yolima</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>hola mundo</t>
   </si>
@@ -36,16 +33,28 @@
     <t>hola</t>
   </si>
   <si>
-    <t>ggg</t>
-  </si>
-  <si>
-    <t>rr</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>e</t>
+    <t>mundo</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>mary</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>ii</t>
+  </si>
+  <si>
+    <t>0.999</t>
   </si>
 </sst>
 </file>
@@ -363,49 +372,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1">
+        <v>0.78</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B4" t="s">
         <v>6</v>
+      </c>
+      <c r="C4">
+        <v>67</v>
+      </c>
+      <c r="D4">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>